<commit_message>
Atualizacao do dashboard de imunizacao
</commit_message>
<xml_diff>
--- a/Gestão do Projeto/DashboardImunizacao.xlsx
+++ b/Gestão do Projeto/DashboardImunizacao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GOInterop\git\HSL-IPS\Gestão do Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD831B8-3979-4468-A389-006C442152BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50488EBD-D30A-4C80-9E90-0F0971F41A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -980,8 +980,8 @@
   </sheetPr>
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23:O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1061,43 +1061,43 @@
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="33">
-        <f>COUNTIF(J4:J17, "TRUE")/(COUNTIF(J4:J17, "TRUE")+COUNTIF(J4:J17, "FALSE"))</f>
+        <f t="shared" ref="J2:S2" si="0">COUNTIF(J4:J17, "TRUE")/(COUNTIF(J4:J17, "TRUE")+COUNTIF(J4:J17, "FALSE"))</f>
+        <v>0.75</v>
+      </c>
+      <c r="K2" s="34">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="L2" s="34">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="K2" s="34">
-        <f>COUNTIF(K4:K17, "TRUE")/(COUNTIF(K4:K17, "TRUE")+COUNTIF(K4:K17, "FALSE"))</f>
+      <c r="M2" s="34">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="L2" s="34">
-        <f>COUNTIF(L4:L17, "TRUE")/(COUNTIF(L4:L17, "TRUE")+COUNTIF(L4:L17, "FALSE"))</f>
+      <c r="N2" s="34">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="M2" s="34">
-        <f>COUNTIF(M4:M17, "TRUE")/(COUNTIF(M4:M17, "TRUE")+COUNTIF(M4:M17, "FALSE"))</f>
+      <c r="O2" s="34">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="N2" s="34">
-        <f>COUNTIF(N4:N17, "TRUE")/(COUNTIF(N4:N17, "TRUE")+COUNTIF(N4:N17, "FALSE"))</f>
+      <c r="P2" s="34">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="O2" s="34">
-        <f>COUNTIF(O4:O17, "TRUE")/(COUNTIF(O4:O17, "TRUE")+COUNTIF(O4:O17, "FALSE"))</f>
+      <c r="Q2" s="34">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="P2" s="34">
-        <f>COUNTIF(P4:P17, "TRUE")/(COUNTIF(P4:P17, "TRUE")+COUNTIF(P4:P17, "FALSE"))</f>
-        <v>0.6</v>
-      </c>
-      <c r="Q2" s="34">
-        <f>COUNTIF(Q4:Q17, "TRUE")/(COUNTIF(Q4:Q17, "TRUE")+COUNTIF(Q4:Q17, "FALSE"))</f>
-        <v>0.6</v>
-      </c>
       <c r="R2" s="34">
-        <f>COUNTIF(R4:R17, "TRUE")/(COUNTIF(R4:R17, "TRUE")+COUNTIF(R4:R17, "FALSE"))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S2" s="34">
-        <f>COUNTIF(S4:S17, "TRUE")/(COUNTIF(S4:S17, "TRUE")+COUNTIF(S4:S17, "FALSE"))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T2" s="38">
@@ -1193,12 +1193,8 @@
       <c r="I4" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="17" t="b">
-        <v>0</v>
-      </c>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
       <c r="L4" s="17" t="b">
         <v>0</v>
       </c>
@@ -1287,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="T5" s="36">
-        <f t="shared" ref="T5:T17" si="0">COUNTIF(J5:S5,"TRUE")/(COUNTIF(J5:S5,"TRUE")+COUNTIF(J5:S5,"FALSE"))</f>
+        <f t="shared" ref="T5:T15" si="1">COUNTIF(J5:S5,"TRUE")/(COUNTIF(J5:S5,"TRUE")+COUNTIF(J5:S5,"FALSE"))</f>
         <v>0.8</v>
       </c>
     </row>
@@ -1494,7 +1490,7 @@
         <v>0</v>
       </c>
       <c r="T10" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1665,7 +1661,7 @@
         <v>0</v>
       </c>
       <c r="T14" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
     </row>
@@ -1728,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="T15" s="36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
     </row>

</xml_diff>